<commit_message>
second commit, update data
</commit_message>
<xml_diff>
--- a/KNN/data.xlsx
+++ b/KNN/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="19">
   <si>
     <t>Возраст</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Экстраверт</t>
   </si>
   <si>
-    <t>Не доволен</t>
-  </si>
-  <si>
     <t>Сова</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>м</t>
   </si>
   <si>
-    <t>Дом</t>
-  </si>
-  <si>
     <t>Да</t>
   </si>
   <si>
@@ -76,12 +70,21 @@
   </si>
   <si>
     <t>Присутствие</t>
+  </si>
+  <si>
+    <t>Дом_далеко</t>
+  </si>
+  <si>
+    <t>Недоволен</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -393,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,25 +422,25 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -444,28 +448,28 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -473,28 +477,28 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -502,28 +506,28 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -531,28 +535,28 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -560,28 +564,28 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>11</v>
       </c>
       <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -589,28 +593,28 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -618,28 +622,28 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -647,28 +651,28 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>9</v>
       </c>
       <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -676,28 +680,28 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>11</v>
       </c>
       <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -705,28 +709,86 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
         <v>7.5</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
       <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="H11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" t="s">
-        <v>15</v>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>